<commit_message>
Updated excel file w/ seperated keywords
</commit_message>
<xml_diff>
--- a/news and keywords.xlsx
+++ b/news and keywords.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\poli-179\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70E24D2-BA5B-451A-BEDA-59E0AC228ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50A1060-21E2-441C-B8DD-96E75842B368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5475" yWindow="225" windowWidth="18060" windowHeight="13380" xr2:uid="{616D4539-124B-419A-916B-006AF051180A}"/>
+    <workbookView xWindow="5475" yWindow="120" windowWidth="18060" windowHeight="13380" xr2:uid="{616D4539-124B-419A-916B-006AF051180A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="144">
   <si>
     <t>News Sites</t>
   </si>
@@ -402,6 +402,72 @@
   </si>
   <si>
     <t>gaza</t>
+  </si>
+  <si>
+    <t>News Sites (v2)</t>
+  </si>
+  <si>
+    <t>apnews</t>
+  </si>
+  <si>
+    <t>nbcnews</t>
+  </si>
+  <si>
+    <t>Keywords (students)</t>
+  </si>
+  <si>
+    <t>Keywords (protest)</t>
+  </si>
+  <si>
+    <t>Keywords (context)</t>
+  </si>
+  <si>
+    <t>student.*</t>
+  </si>
+  <si>
+    <t>campus.*</t>
+  </si>
+  <si>
+    <t>universit.*</t>
+  </si>
+  <si>
+    <t>college.*</t>
+  </si>
+  <si>
+    <t>school.*</t>
+  </si>
+  <si>
+    <t>faculty.*</t>
+  </si>
+  <si>
+    <t>activis.*</t>
+  </si>
+  <si>
+    <t>protest.*</t>
+  </si>
+  <si>
+    <t>encamp.*</t>
+  </si>
+  <si>
+    <t>demonstrat.*</t>
+  </si>
+  <si>
+    <t>clash.*</t>
+  </si>
+  <si>
+    <t>divest.*</t>
+  </si>
+  <si>
+    <t>war.*</t>
+  </si>
+  <si>
+    <t>palestin.*</t>
+  </si>
+  <si>
+    <t>israel.*</t>
+  </si>
+  <si>
+    <t>arrest.*</t>
   </si>
 </sst>
 </file>
@@ -773,552 +839,643 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545A83E4-D46F-4926-B5C1-7D21E1312B38}">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
         <v>41</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>42</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
         <v>109</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>46</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>47</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>48</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>51</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>50</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>52</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>53</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>54</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>55</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>56</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>57</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>58</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>59</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>60</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>61</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>100</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>101</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>102</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>103</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>104</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated excel file w/ wip politcal leanings and test run of analysis on test data
</commit_message>
<xml_diff>
--- a/news and keywords.xlsx
+++ b/news and keywords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\poli-179\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50A1060-21E2-441C-B8DD-96E75842B368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EB33F8-6D51-4D39-810B-144276C84D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5475" yWindow="120" windowWidth="18060" windowHeight="13380" xr2:uid="{616D4539-124B-419A-916B-006AF051180A}"/>
+    <workbookView xWindow="3600" yWindow="1185" windowWidth="9615" windowHeight="13380" xr2:uid="{616D4539-124B-419A-916B-006AF051180A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="159">
   <si>
     <t>News Sites</t>
   </si>
@@ -468,6 +468,51 @@
   </si>
   <si>
     <t>arrest.*</t>
+  </si>
+  <si>
+    <t>abcnews.go</t>
+  </si>
+  <si>
+    <t>cbsnews</t>
+  </si>
+  <si>
+    <t>foxnews</t>
+  </si>
+  <si>
+    <t>nytimes</t>
+  </si>
+  <si>
+    <t>usatoday</t>
+  </si>
+  <si>
+    <t>vice</t>
+  </si>
+  <si>
+    <t>buzzfeednews</t>
+  </si>
+  <si>
+    <t>businessinsider</t>
+  </si>
+  <si>
+    <t>huffpost</t>
+  </si>
+  <si>
+    <t>thehill</t>
+  </si>
+  <si>
+    <t>aljazeera</t>
+  </si>
+  <si>
+    <t>hamas</t>
+  </si>
+  <si>
+    <t>theguardian</t>
+  </si>
+  <si>
+    <t>news.sky</t>
+  </si>
+  <si>
+    <t>Score (v2)</t>
   </si>
 </sst>
 </file>
@@ -839,24 +884,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545A83E4-D46F-4926-B5C1-7D21E1312B38}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -864,618 +909,759 @@
         <v>122</v>
       </c>
       <c r="C1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>111</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>125</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>126</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>112</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>109</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>134</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>123</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>40</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>128</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>135</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>107</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>130</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>136</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5" t="s">
         <v>44</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>108</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>131</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>137</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>124</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6" t="s">
         <v>45</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>113</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>132</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <v>-1</v>
+      </c>
+      <c r="D7" t="s">
         <v>109</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>106</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>129</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8">
+        <v>-1</v>
+      </c>
+      <c r="D8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>54</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>133</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9">
+        <v>-1</v>
+      </c>
+      <c r="D9" t="s">
         <v>47</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>55</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>48</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" t="s">
         <v>49</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" t="s">
         <v>51</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" t="s">
         <v>50</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>-1</v>
+      </c>
+      <c r="D14" t="s">
         <v>52</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
         <v>53</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" t="s">
         <v>54</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="C17" t="s">
+      <c r="B17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" t="s">
         <v>55</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="C18" t="s">
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <v>-1</v>
+      </c>
+      <c r="D18" t="s">
         <v>56</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" t="s">
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
         <v>57</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
+      <c r="B20" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20">
+        <v>-1</v>
+      </c>
+      <c r="D20" t="s">
         <v>58</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
         <v>59</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="C22" t="s">
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" t="s">
         <v>60</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="C23" t="s">
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
         <v>61</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="C24" t="s">
+      <c r="B24" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="C25" t="s">
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25">
+        <v>-1</v>
+      </c>
+      <c r="D25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="C26" t="s">
+      <c r="B26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="C27" t="s">
+      <c r="B27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27">
+        <v>-1</v>
+      </c>
+      <c r="D27" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="C28" t="s">
+      <c r="B28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28">
+        <v>-1</v>
+      </c>
+      <c r="D28" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="C29" t="s">
+      <c r="B29" t="s">
+        <v>156</v>
+      </c>
+      <c r="C29">
+        <v>-1</v>
+      </c>
+      <c r="D29" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="C30" t="s">
+      <c r="B30" t="s">
+        <v>157</v>
+      </c>
+      <c r="D30" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
-      <c r="C31" t="s">
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>-1</v>
+      </c>
+      <c r="D31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>100</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>101</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>102</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>103</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>104</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C62" t="s">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C63" t="s">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C64" t="s">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Excel file w/leaning scores for news sites
</commit_message>
<xml_diff>
--- a/news and keywords.xlsx
+++ b/news and keywords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\poli-179\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EB33F8-6D51-4D39-810B-144276C84D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92542EBD-676C-4864-8FBD-7631AD351537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="1185" windowWidth="9615" windowHeight="13380" xr2:uid="{616D4539-124B-419A-916B-006AF051180A}"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="9615" windowHeight="13380" xr2:uid="{616D4539-124B-419A-916B-006AF051180A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="162">
   <si>
     <t>News Sites</t>
   </si>
@@ -513,6 +513,15 @@
   </si>
   <si>
     <t>Score (v2)</t>
+  </si>
+  <si>
+    <t>washingtonpost</t>
+  </si>
+  <si>
+    <t>pbs</t>
+  </si>
+  <si>
+    <t>economist</t>
   </si>
 </sst>
 </file>
@@ -886,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545A83E4-D46F-4926-B5C1-7D21E1312B38}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +970,7 @@
         <v>123</v>
       </c>
       <c r="C3">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="D3" t="s">
         <v>41</v>
@@ -987,7 +996,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D4" t="s">
         <v>42</v>
@@ -1013,7 +1022,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="D5" t="s">
         <v>44</v>
@@ -1085,7 +1094,7 @@
         <v>144</v>
       </c>
       <c r="C8">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="D8" t="s">
         <v>46</v>
@@ -1108,7 +1117,7 @@
         <v>145</v>
       </c>
       <c r="C9">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="D9" t="s">
         <v>47</v>
@@ -1144,6 +1153,9 @@
       <c r="B11" t="s">
         <v>147</v>
       </c>
+      <c r="C11">
+        <v>-1</v>
+      </c>
       <c r="D11" t="s">
         <v>49</v>
       </c>
@@ -1158,6 +1170,9 @@
       <c r="B12" t="s">
         <v>148</v>
       </c>
+      <c r="C12">
+        <v>-0.5</v>
+      </c>
       <c r="D12" t="s">
         <v>51</v>
       </c>
@@ -1172,6 +1187,9 @@
       <c r="B13" t="s">
         <v>149</v>
       </c>
+      <c r="C13">
+        <v>-1</v>
+      </c>
       <c r="D13" t="s">
         <v>50</v>
       </c>
@@ -1203,6 +1221,9 @@
       <c r="B15" t="s">
         <v>24</v>
       </c>
+      <c r="C15">
+        <v>-0.5</v>
+      </c>
       <c r="D15" t="s">
         <v>53</v>
       </c>
@@ -1231,6 +1252,9 @@
       <c r="B17" t="s">
         <v>151</v>
       </c>
+      <c r="C17">
+        <v>-0.5</v>
+      </c>
       <c r="D17" t="s">
         <v>55</v>
       </c>
@@ -1246,7 +1270,7 @@
         <v>27</v>
       </c>
       <c r="C18">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="D18" t="s">
         <v>56</v>
@@ -1263,7 +1287,7 @@
         <v>29</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="D19" t="s">
         <v>57</v>
@@ -1297,7 +1321,7 @@
         <v>32</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="D21" t="s">
         <v>59</v>
@@ -1311,7 +1335,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>159</v>
+      </c>
+      <c r="C22">
+        <v>-1</v>
       </c>
       <c r="D22" t="s">
         <v>60</v>
@@ -1344,6 +1371,9 @@
       <c r="B24" t="s">
         <v>153</v>
       </c>
+      <c r="C24">
+        <v>-0.5</v>
+      </c>
       <c r="D24" t="s">
         <v>62</v>
       </c>
@@ -1373,7 +1403,7 @@
         <v>102</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="D26" t="s">
         <v>64</v>
@@ -1401,7 +1431,7 @@
         <v>104</v>
       </c>
       <c r="C28">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="D28" t="s">
         <v>66</v>
@@ -1428,6 +1458,9 @@
       <c r="B30" t="s">
         <v>157</v>
       </c>
+      <c r="C30">
+        <v>-0.5</v>
+      </c>
       <c r="D30" t="s">
         <v>68</v>
       </c>
@@ -1450,6 +1483,12 @@
       <c r="A32" t="s">
         <v>32</v>
       </c>
+      <c r="B32" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32">
+        <v>-0.5</v>
+      </c>
       <c r="D32" t="s">
         <v>70</v>
       </c>
@@ -1457,6 +1496,12 @@
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>161</v>
+      </c>
+      <c r="C33">
+        <v>-0.5</v>
       </c>
       <c r="D33" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Added more right leaning outlets
</commit_message>
<xml_diff>
--- a/news and keywords.xlsx
+++ b/news and keywords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\poli-179\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92542EBD-676C-4864-8FBD-7631AD351537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000DAE53-52B4-4C81-8687-11CD6699C19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="9615" windowHeight="13380" xr2:uid="{616D4539-124B-419A-916B-006AF051180A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{616D4539-124B-419A-916B-006AF051180A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="176">
   <si>
     <t>News Sites</t>
   </si>
@@ -522,6 +522,48 @@
   </si>
   <si>
     <t>economist</t>
+  </si>
+  <si>
+    <t>nationalreview</t>
+  </si>
+  <si>
+    <t>breitbart</t>
+  </si>
+  <si>
+    <t>hannity</t>
+  </si>
+  <si>
+    <t>theblaze</t>
+  </si>
+  <si>
+    <t>heritage</t>
+  </si>
+  <si>
+    <t>washingtonexaminer</t>
+  </si>
+  <si>
+    <t>dailywire</t>
+  </si>
+  <si>
+    <t>thefederalist</t>
+  </si>
+  <si>
+    <t>thegatewaypundit</t>
+  </si>
+  <si>
+    <t>dailycaller</t>
+  </si>
+  <si>
+    <t>infowars</t>
+  </si>
+  <si>
+    <t>stanfordreview</t>
+  </si>
+  <si>
+    <t>thenewamerican</t>
+  </si>
+  <si>
+    <t>prntly</t>
   </si>
 </sst>
 </file>
@@ -896,7 +938,7 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,6 +1553,12 @@
       <c r="A34" t="s">
         <v>34</v>
       </c>
+      <c r="B34" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
       <c r="D34" t="s">
         <v>72</v>
       </c>
@@ -1519,6 +1567,12 @@
       <c r="A35" t="s">
         <v>35</v>
       </c>
+      <c r="B35" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
       <c r="D35" t="s">
         <v>73</v>
       </c>
@@ -1527,6 +1581,12 @@
       <c r="A36" t="s">
         <v>36</v>
       </c>
+      <c r="B36" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
       <c r="D36" t="s">
         <v>74</v>
       </c>
@@ -1535,6 +1595,12 @@
       <c r="A37" t="s">
         <v>37</v>
       </c>
+      <c r="B37" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
       <c r="D37" t="s">
         <v>75</v>
       </c>
@@ -1543,6 +1609,12 @@
       <c r="A38" t="s">
         <v>38</v>
       </c>
+      <c r="B38" t="s">
+        <v>166</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
       <c r="D38" t="s">
         <v>76</v>
       </c>
@@ -1551,6 +1623,12 @@
       <c r="A39" t="s">
         <v>39</v>
       </c>
+      <c r="B39" t="s">
+        <v>167</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
       <c r="D39" t="s">
         <v>77</v>
       </c>
@@ -1559,6 +1637,12 @@
       <c r="A40" t="s">
         <v>100</v>
       </c>
+      <c r="B40" t="s">
+        <v>168</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
       <c r="D40" t="s">
         <v>78</v>
       </c>
@@ -1567,6 +1651,12 @@
       <c r="A41" t="s">
         <v>101</v>
       </c>
+      <c r="B41" t="s">
+        <v>169</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
       <c r="D41" t="s">
         <v>79</v>
       </c>
@@ -1575,6 +1665,12 @@
       <c r="A42" t="s">
         <v>102</v>
       </c>
+      <c r="B42" t="s">
+        <v>170</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
       <c r="D42" t="s">
         <v>110</v>
       </c>
@@ -1583,6 +1679,12 @@
       <c r="A43" t="s">
         <v>103</v>
       </c>
+      <c r="B43" t="s">
+        <v>171</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
       <c r="D43" t="s">
         <v>80</v>
       </c>
@@ -1591,21 +1693,45 @@
       <c r="A44" t="s">
         <v>104</v>
       </c>
+      <c r="B44" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
       <c r="D44" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>173</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
       <c r="D45" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>174</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
       <c r="D46" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>175</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
       <c r="D47" t="s">
         <v>84</v>
       </c>

</xml_diff>